<commit_message>
Largest Rectangle in Histogram - 설명 수정
</commit_message>
<xml_diff>
--- a/src/main/kotlin/com/leetcode/P84.xlsx
+++ b/src/main/kotlin/com/leetcode/P84.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\projects\algorithm\src\main\java\com\leetcode\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\projects\algorithm\src\main\kotlin\com\leetcode\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3E65F5F3-1756-48D5-B49B-CE5A9C665489}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{930E42AE-FE0E-41A4-A789-881C24790C6C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="12735" yWindow="1470" windowWidth="15450" windowHeight="12195" xr2:uid="{61816CE9-7D59-4EEA-8AFD-F9EFEA061734}"/>
   </bookViews>
@@ -85,7 +85,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -145,13 +145,62 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -170,31 +219,49 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -514,7 +581,7 @@
   <dimension ref="B2:AI16"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="O17" sqref="O17"/>
+      <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.625" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -540,45 +607,48 @@
     </row>
     <row r="6" spans="2:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
-      <c r="D6" s="12"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="12"/>
-      <c r="L6" s="11"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="9"/>
+      <c r="G6" s="8"/>
+      <c r="L6" s="7"/>
     </row>
     <row r="7" spans="2:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B7" s="3"/>
       <c r="C7" s="4"/>
-      <c r="D7" s="14"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="14"/>
-      <c r="G7" s="14"/>
+      <c r="D7" s="10"/>
+      <c r="E7" s="10"/>
+      <c r="F7" s="10"/>
+      <c r="G7" s="10"/>
     </row>
     <row r="8" spans="2:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="10">
-        <v>2</v>
-      </c>
-      <c r="C8" s="10">
+      <c r="B8" s="6">
+        <v>2</v>
+      </c>
+      <c r="C8" s="6">
         <v>1</v>
       </c>
-      <c r="D8" s="10">
+      <c r="D8" s="6">
         <v>5</v>
       </c>
-      <c r="E8" s="10">
+      <c r="E8" s="6">
         <v>6</v>
       </c>
       <c r="F8" s="1">
         <v>2</v>
       </c>
-      <c r="G8" s="1">
+      <c r="G8" s="6">
         <v>3</v>
       </c>
     </row>
     <row r="10" spans="2:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="E10" s="2"/>
       <c r="L10" s="2"/>
+      <c r="R10" s="20"/>
       <c r="S10" s="2"/>
-      <c r="Z10" s="7"/>
+      <c r="Z10" s="11">
+        <v>6</v>
+      </c>
       <c r="AG10" s="2"/>
     </row>
     <row r="11" spans="2:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
@@ -586,10 +656,12 @@
       <c r="E11" s="5"/>
       <c r="K11" s="2"/>
       <c r="L11" s="5"/>
-      <c r="R11" s="7"/>
-      <c r="S11" s="6"/>
+      <c r="R11" s="14">
+        <v>10</v>
+      </c>
+      <c r="S11" s="16"/>
       <c r="Y11" s="2"/>
-      <c r="Z11" s="6"/>
+      <c r="Z11" s="13"/>
       <c r="AF11" s="2"/>
       <c r="AG11" s="5"/>
     </row>
@@ -598,80 +670,90 @@
       <c r="E12" s="5"/>
       <c r="K12" s="5"/>
       <c r="L12" s="5"/>
-      <c r="R12" s="6"/>
-      <c r="S12" s="6"/>
+      <c r="R12" s="14"/>
+      <c r="S12" s="16"/>
       <c r="Y12" s="5"/>
-      <c r="Z12" s="6"/>
+      <c r="Z12" s="13"/>
       <c r="AF12" s="5"/>
       <c r="AG12" s="5"/>
     </row>
     <row r="13" spans="2:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D13" s="5"/>
       <c r="E13" s="5"/>
+      <c r="F13" s="3"/>
       <c r="G13" s="2"/>
       <c r="K13" s="5"/>
       <c r="L13" s="5"/>
       <c r="N13" s="2"/>
-      <c r="R13" s="6"/>
-      <c r="S13" s="6"/>
+      <c r="R13" s="14"/>
+      <c r="S13" s="16"/>
       <c r="U13" s="2"/>
       <c r="Y13" s="5"/>
-      <c r="Z13" s="6"/>
+      <c r="Z13" s="13"/>
       <c r="AB13" s="2"/>
       <c r="AF13" s="5"/>
       <c r="AG13" s="5"/>
-      <c r="AI13" s="7"/>
+      <c r="AI13" s="11">
+        <v>3</v>
+      </c>
     </row>
     <row r="14" spans="2:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="2"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="7"/>
-      <c r="G14" s="6"/>
+      <c r="B14" s="11">
+        <v>2</v>
+      </c>
+      <c r="D14" s="14">
+        <v>8</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="16"/>
       <c r="I14" s="2"/>
+      <c r="J14" s="3"/>
       <c r="K14" s="5"/>
       <c r="L14" s="5"/>
       <c r="M14" s="2"/>
       <c r="N14" s="5"/>
       <c r="P14" s="2"/>
-      <c r="R14" s="6"/>
-      <c r="S14" s="6"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="16"/>
       <c r="T14" s="2"/>
       <c r="U14" s="5"/>
       <c r="W14" s="2"/>
       <c r="Y14" s="5"/>
-      <c r="Z14" s="6"/>
+      <c r="Z14" s="13"/>
       <c r="AA14" s="2"/>
       <c r="AB14" s="5"/>
       <c r="AD14" s="2"/>
       <c r="AF14" s="5"/>
       <c r="AG14" s="5"/>
       <c r="AH14" s="2"/>
-      <c r="AI14" s="6"/>
+      <c r="AI14" s="13"/>
     </row>
     <row r="15" spans="2:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="3"/>
+      <c r="B15" s="12"/>
       <c r="C15" s="4"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="I15" s="8"/>
-      <c r="J15" s="9"/>
-      <c r="K15" s="8"/>
-      <c r="L15" s="8"/>
-      <c r="M15" s="8"/>
-      <c r="N15" s="8"/>
+      <c r="D15" s="17"/>
+      <c r="E15" s="18"/>
+      <c r="F15" s="18"/>
+      <c r="G15" s="19"/>
+      <c r="I15" s="17">
+        <v>6</v>
+      </c>
+      <c r="J15" s="18"/>
+      <c r="K15" s="18"/>
+      <c r="L15" s="18"/>
+      <c r="M15" s="18"/>
+      <c r="N15" s="19"/>
       <c r="P15" s="3"/>
       <c r="Q15" s="4"/>
-      <c r="R15" s="8"/>
-      <c r="S15" s="8"/>
+      <c r="R15" s="17"/>
+      <c r="S15" s="19"/>
       <c r="T15" s="3"/>
       <c r="U15" s="3"/>
       <c r="W15" s="3"/>
       <c r="X15" s="4"/>
       <c r="Y15" s="3"/>
-      <c r="Z15" s="8"/>
+      <c r="Z15" s="12"/>
       <c r="AA15" s="3"/>
       <c r="AB15" s="3"/>
       <c r="AD15" s="3"/>
@@ -679,10 +761,10 @@
       <c r="AF15" s="3"/>
       <c r="AG15" s="3"/>
       <c r="AH15" s="3"/>
-      <c r="AI15" s="8"/>
+      <c r="AI15" s="12"/>
     </row>
     <row r="16" spans="2:35" ht="15" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="10">
+      <c r="B16" s="6">
         <v>2</v>
       </c>
       <c r="C16" s="1">
@@ -703,7 +785,7 @@
       <c r="I16" s="1">
         <v>2</v>
       </c>
-      <c r="J16" s="10">
+      <c r="J16" s="6">
         <v>1</v>
       </c>
       <c r="K16" s="1">
@@ -724,7 +806,7 @@
       <c r="Q16" s="1">
         <v>1</v>
       </c>
-      <c r="R16" s="10">
+      <c r="R16" s="6">
         <v>5</v>
       </c>
       <c r="S16" s="1">
@@ -745,7 +827,7 @@
       <c r="Y16" s="1">
         <v>5</v>
       </c>
-      <c r="Z16" s="10">
+      <c r="Z16" s="6">
         <v>6</v>
       </c>
       <c r="AA16" s="1">
@@ -769,11 +851,19 @@
       <c r="AH16" s="1">
         <v>2</v>
       </c>
-      <c r="AI16" s="10">
+      <c r="AI16" s="6">
         <v>3</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="6">
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="D14:G15"/>
+    <mergeCell ref="I15:N15"/>
+    <mergeCell ref="R11:S15"/>
+    <mergeCell ref="Z10:Z15"/>
+    <mergeCell ref="AI13:AI15"/>
+  </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>